<commit_message>
codelijst aanvullen met altLabel
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,36 +425,39 @@
         <v>theme</v>
       </c>
       <c r="H1" t="str">
+        <v>altLabel</v>
+      </c>
+      <c r="I1" t="str">
         <v>broader</v>
       </c>
-      <c r="I1" t="str">
+      <c r="J1" t="str">
         <v>broaderTransitive</v>
       </c>
-      <c r="J1" t="str">
+      <c r="K1" t="str">
         <v>semanticRelation</v>
       </c>
-      <c r="K1" t="str">
+      <c r="L1" t="str">
         <v>gekoppelde_eigenschap</v>
       </c>
-      <c r="L1" t="str">
+      <c r="M1" t="str">
         <v>narrower</v>
       </c>
-      <c r="M1" t="str">
+      <c r="N1" t="str">
         <v>narrowerTransitive</v>
       </c>
-      <c r="N1" t="str">
+      <c r="O1" t="str">
         <v>topConceptOf</v>
       </c>
-      <c r="O1" t="str">
+      <c r="P1" t="str">
         <v>belongsTo</v>
       </c>
-      <c r="P1" t="str">
+      <c r="Q1" t="str">
         <v>definition</v>
       </c>
-      <c r="Q1" t="str">
+      <c r="R1" t="str">
         <v>hasTopConcept</v>
       </c>
-      <c r="R1" t="str">
+      <c r="S1" t="str">
         <v>note</v>
       </c>
     </row>
@@ -513,6 +516,9 @@
       <c r="R2" t="str">
         <v>null</v>
       </c>
+      <c r="S2" t="str">
+        <v>null</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -531,13 +537,13 @@
         <v>buitenmuren</v>
       </c>
       <c r="F3" t="str">
-        <v>Gebrek aan de toestand van buitenmuren.</v>
+        <v>Gebrek aan de toestand van buitenmuren</v>
       </c>
       <c r="G3" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H3" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Buitenmuren</v>
       </c>
       <c r="I3" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -546,11 +552,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K3" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L3" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_buitenmuren</v>
       </c>
-      <c r="L3" t="str">
-        <v>null</v>
-      </c>
       <c r="M3" t="str">
         <v>null</v>
       </c>
@@ -567,6 +573,9 @@
         <v>null</v>
       </c>
       <c r="R3" t="str">
+        <v>null</v>
+      </c>
+      <c r="S3" t="str">
         <v>null</v>
       </c>
     </row>
@@ -587,13 +596,13 @@
         <v>buitentimmerwerk</v>
       </c>
       <c r="F4" t="str">
-        <v>Gebrek aan de toestand van het buitentimmerwerk.</v>
+        <v>Gebrek aan de toestand van het buitentimmerwerk</v>
       </c>
       <c r="G4" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H4" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Buitentimmerwerk</v>
       </c>
       <c r="I4" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -602,11 +611,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K4" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L4" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_buitentimmerwerk</v>
       </c>
-      <c r="L4" t="str">
-        <v>null</v>
-      </c>
       <c r="M4" t="str">
         <v>null</v>
       </c>
@@ -623,6 +632,9 @@
         <v>null</v>
       </c>
       <c r="R4" t="str">
+        <v>null</v>
+      </c>
+      <c r="S4" t="str">
         <v>null</v>
       </c>
     </row>
@@ -643,13 +655,13 @@
         <v>dakbedekking</v>
       </c>
       <c r="F5" t="str">
-        <v>Gebrek aan de toestand van de dakbedekking.</v>
+        <v>Gebrek aan de toestand van de dakbedekking</v>
       </c>
       <c r="G5" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H5" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Dakbedekking</v>
       </c>
       <c r="I5" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -658,11 +670,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K5" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L5" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakbedekking</v>
       </c>
-      <c r="L5" t="str">
-        <v>null</v>
-      </c>
       <c r="M5" t="str">
         <v>null</v>
       </c>
@@ -679,6 +691,9 @@
         <v>null</v>
       </c>
       <c r="R5" t="str">
+        <v>null</v>
+      </c>
+      <c r="S5" t="str">
         <v>null</v>
       </c>
     </row>
@@ -699,13 +714,13 @@
         <v>dakgebinte</v>
       </c>
       <c r="F6" t="str">
-        <v>Gebrek aan de toestand van het dakgebinte.</v>
+        <v>Gebrek aan de toestand van het dakgebinte</v>
       </c>
       <c r="G6" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H6" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Dakgebinte</v>
       </c>
       <c r="I6" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -714,11 +729,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K6" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L6" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakgebinte</v>
       </c>
-      <c r="L6" t="str">
-        <v>null</v>
-      </c>
       <c r="M6" t="str">
         <v>null</v>
       </c>
@@ -735,6 +750,9 @@
         <v>null</v>
       </c>
       <c r="R6" t="str">
+        <v>null</v>
+      </c>
+      <c r="S6" t="str">
         <v>null</v>
       </c>
     </row>
@@ -755,13 +773,13 @@
         <v>dakgoten</v>
       </c>
       <c r="F7" t="str">
-        <v>Gebrek aan de toestand van de dakgoten.</v>
+        <v>Gebrek aan de toestand van de dakgoten</v>
       </c>
       <c r="G7" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H7" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Dakgoten</v>
       </c>
       <c r="I7" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -770,11 +788,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K7" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L7" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakgoten</v>
       </c>
-      <c r="L7" t="str">
-        <v>null</v>
-      </c>
       <c r="M7" t="str">
         <v>null</v>
       </c>
@@ -791,6 +809,9 @@
         <v>null</v>
       </c>
       <c r="R7" t="str">
+        <v>null</v>
+      </c>
+      <c r="S7" t="str">
         <v>null</v>
       </c>
     </row>
@@ -811,34 +832,34 @@
         <v>gebouwonderdeel</v>
       </c>
       <c r="F8" t="str">
-        <v>Gebrek aan de toestand van een gebouwonderdeel.</v>
+        <v>Gebrek aan de toestand van een gebouwonderdeel</v>
       </c>
       <c r="G8" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H8" t="str">
-        <v>null</v>
+        <v>Gebrek aan de toestand van een gebouwonderdeel</v>
       </c>
       <c r="I8" t="str">
         <v>null</v>
       </c>
       <c r="J8" t="str">
+        <v>null</v>
+      </c>
+      <c r="K8" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/liften|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/trappen</v>
       </c>
-      <c r="K8" t="str">
+      <c r="L8" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_gebouwonderdeel</v>
-      </c>
-      <c r="L8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/liften|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/trappen</v>
       </c>
       <c r="M8" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/liften|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/trappen</v>
       </c>
       <c r="N8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/verwaarlozing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/liften|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/trappen</v>
       </c>
       <c r="O8" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/verwaarlozing</v>
       </c>
       <c r="P8" t="str">
         <v>null</v>
@@ -847,6 +868,9 @@
         <v>null</v>
       </c>
       <c r="R8" t="str">
+        <v>null</v>
+      </c>
+      <c r="S8" t="str">
         <v>null</v>
       </c>
     </row>
@@ -867,13 +891,13 @@
         <v>kroonlijst</v>
       </c>
       <c r="F9" t="str">
-        <v>Gebrek aan de toestand van de kroonlijst.</v>
+        <v>Gebrek aan de toestand van de kroonlijst</v>
       </c>
       <c r="G9" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H9" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Kroonlijst</v>
       </c>
       <c r="I9" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -882,11 +906,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K9" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L9" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_kroonlijst</v>
       </c>
-      <c r="L9" t="str">
-        <v>null</v>
-      </c>
       <c r="M9" t="str">
         <v>null</v>
       </c>
@@ -903,6 +927,9 @@
         <v>null</v>
       </c>
       <c r="R9" t="str">
+        <v>null</v>
+      </c>
+      <c r="S9" t="str">
         <v>null</v>
       </c>
     </row>
@@ -923,13 +950,13 @@
         <v>liften</v>
       </c>
       <c r="F10" t="str">
-        <v>Gebrek aan de toestand van de liften.</v>
+        <v>Gebrek aan de toestand van de liften</v>
       </c>
       <c r="G10" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H10" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Liften</v>
       </c>
       <c r="I10" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -938,11 +965,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K10" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L10" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_liften</v>
       </c>
-      <c r="L10" t="str">
-        <v>null</v>
-      </c>
       <c r="M10" t="str">
         <v>null</v>
       </c>
@@ -959,6 +986,9 @@
         <v>null</v>
       </c>
       <c r="R10" t="str">
+        <v>null</v>
+      </c>
+      <c r="S10" t="str">
         <v>null</v>
       </c>
     </row>
@@ -979,13 +1009,13 @@
         <v>schoorstenen</v>
       </c>
       <c r="F11" t="str">
-        <v>Gebrek aan de toestand van schoorstenen.</v>
+        <v>Gebrek aan de toestand van schoorstenen</v>
       </c>
       <c r="G11" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Schoorstenen</v>
       </c>
       <c r="I11" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -994,11 +1024,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K11" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L11" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_schoorstenen</v>
       </c>
-      <c r="L11" t="str">
-        <v>null</v>
-      </c>
       <c r="M11" t="str">
         <v>null</v>
       </c>
@@ -1015,6 +1045,9 @@
         <v>null</v>
       </c>
       <c r="R11" t="str">
+        <v>null</v>
+      </c>
+      <c r="S11" t="str">
         <v>null</v>
       </c>
     </row>
@@ -1035,13 +1068,13 @@
         <v>stabiliteit</v>
       </c>
       <c r="F12" t="str">
-        <v>Gebrek dat stabiliteit in het gedrang brengt.</v>
+        <v>Gebrek dat stabiliteit in het gedrang brengt</v>
       </c>
       <c r="G12" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H12" t="str">
-        <v>null</v>
+        <v>Gebrek dat stabiliteit in het gedrang brengt</v>
       </c>
       <c r="I12" t="str">
         <v>null</v>
@@ -1050,19 +1083,19 @@
         <v>null</v>
       </c>
       <c r="K12" t="str">
+        <v>null</v>
+      </c>
+      <c r="L12" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_stabiliteit</v>
       </c>
-      <c r="L12" t="str">
-        <v>null</v>
-      </c>
       <c r="M12" t="str">
         <v>null</v>
       </c>
       <c r="N12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/verwaarlozing</v>
+        <v>null</v>
       </c>
       <c r="O12" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/verwaarlozing</v>
       </c>
       <c r="P12" t="str">
         <v>null</v>
@@ -1071,6 +1104,9 @@
         <v>null</v>
       </c>
       <c r="R12" t="str">
+        <v>null</v>
+      </c>
+      <c r="S12" t="str">
         <v>null</v>
       </c>
     </row>
@@ -1091,13 +1127,13 @@
         <v>trappen</v>
       </c>
       <c r="F13" t="str">
-        <v>Gebrek aan de toestand van de trappen.</v>
+        <v>Gebrek aan de toestand van de trappen</v>
       </c>
       <c r="G13" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+        <v>Trappen</v>
       </c>
       <c r="I13" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
@@ -1106,11 +1142,11 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
       </c>
       <c r="K13" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel</v>
+      </c>
+      <c r="L13" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_trappen</v>
       </c>
-      <c r="L13" t="str">
-        <v>null</v>
-      </c>
       <c r="M13" t="str">
         <v>null</v>
       </c>
@@ -1127,6 +1163,9 @@
         <v>null</v>
       </c>
       <c r="R13" t="str">
+        <v>null</v>
+      </c>
+      <c r="S13" t="str">
         <v>null</v>
       </c>
     </row>
@@ -1147,13 +1186,13 @@
         <v>veiligheid</v>
       </c>
       <c r="F14" t="str">
-        <v>Gebrek dat veiligheid in het gedrang brengt.</v>
+        <v>Gebrek dat veiligheid in het gedrang brengt</v>
       </c>
       <c r="G14" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H14" t="str">
-        <v>null</v>
+        <v>Gebrek dat veiligheid in het gedrang brengt</v>
       </c>
       <c r="I14" t="str">
         <v>null</v>
@@ -1162,19 +1201,19 @@
         <v>null</v>
       </c>
       <c r="K14" t="str">
+        <v>null</v>
+      </c>
+      <c r="L14" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_veiligheid</v>
       </c>
-      <c r="L14" t="str">
-        <v>null</v>
-      </c>
       <c r="M14" t="str">
         <v>null</v>
       </c>
       <c r="N14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/verwaarlozing</v>
+        <v>null</v>
       </c>
       <c r="O14" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/verwaarlozing</v>
       </c>
       <c r="P14" t="str">
         <v>null</v>
@@ -1183,6 +1222,9 @@
         <v>null</v>
       </c>
       <c r="R14" t="str">
+        <v>null</v>
+      </c>
+      <c r="S14" t="str">
         <v>null</v>
       </c>
     </row>
@@ -1203,13 +1245,13 @@
         <v>vochtindringing</v>
       </c>
       <c r="F15" t="str">
-        <v>Gebrek dat leidt tot vochtindringing.</v>
+        <v>Gebrek dat leidt tot vochtindringing</v>
       </c>
       <c r="G15" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="H15" t="str">
-        <v>null</v>
+        <v>Gebrek dat leidt tot vochtindringing</v>
       </c>
       <c r="I15" t="str">
         <v>null</v>
@@ -1218,19 +1260,19 @@
         <v>null</v>
       </c>
       <c r="K15" t="str">
+        <v>null</v>
+      </c>
+      <c r="L15" t="str">
         <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_vochtindringing</v>
       </c>
-      <c r="L15" t="str">
-        <v>null</v>
-      </c>
       <c r="M15" t="str">
         <v>null</v>
       </c>
       <c r="N15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/verwaarlozing</v>
+        <v>null</v>
       </c>
       <c r="O15" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/verwaarlozing</v>
       </c>
       <c r="P15" t="str">
         <v>null</v>
@@ -1239,6 +1281,9 @@
         <v>null</v>
       </c>
       <c r="R15" t="str">
+        <v>null</v>
+      </c>
+      <c r="S15" t="str">
         <v>null</v>
       </c>
     </row>
@@ -1286,21 +1331,24 @@
         <v>null</v>
       </c>
       <c r="O16" t="str">
+        <v>null</v>
+      </c>
+      <c r="P16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-verwaarlozing</v>
       </c>
-      <c r="P16" t="str">
+      <c r="Q16" t="str">
         <v>Het vertonen van uitgesproken gebreken van algemene of beperkte omvang van bedrijfsverwaarlozing. De Vlaamse regering bepaalt de gebreken van algemene en beperkte omvang, alsook de criteria voor de beoordeling van de gebreken en de minimumnorm van de te vertonen gebreken om een bedrijfsruimte al dan niet als geheel of gedeeltelijk verwaarloosd te beschouwen;</v>
       </c>
-      <c r="Q16" t="str">
+      <c r="R16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/gebouwonderdeel|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/stabiliteit|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/veiligheid|https://data.omgeving.vlaanderen.be/id/concept/verwaarlozing/vochtindringing</v>
       </c>
-      <c r="R16" t="str">
+      <c r="S16" t="str">
         <v>Het vertonen van uitgesproken gebreken van algemene of beperkte omvang van bedrijfsverwaarlozing. De Vlaamse regering bepaalt de gebreken van algemene en beperkte omvang, alsook de criteria voor de beoordeling van de gebreken en de minimumnorm van de te vertonen gebreken om een bedrijfsruimte al dan niet als geheel of gedeeltelijk verwaarloosd te beschouwen;</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:R16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LVBR-293 Aanmaken / aanpassen codelijsten voor LVBR
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
@@ -891,7 +891,7 @@
         <v>geregistreerd_in_inventaris</v>
       </c>
       <c r="F9" t="str">
-        <v>geregistreerd in inventaris</v>
+        <v>Geregistreerd in inventaris</v>
       </c>
       <c r="G9" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/beslissing</v>
@@ -1068,7 +1068,7 @@
         <v>niet_geregistreerd_in_inventaris</v>
       </c>
       <c r="F12" t="str">
-        <v>niet_geregistreerd_in_inventaris</v>
+        <v>Niet geregistreerd in inventaris</v>
       </c>
       <c r="G12" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/beslissing</v>

</xml_diff>

<commit_message>
typo fixen en preflabels invullen
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
@@ -478,7 +478,7 @@
         <v>aanvraag_opschorting_heffing_aanvaard</v>
       </c>
       <c r="F2" t="str">
-        <v>aanvraag_opschorting_heffing_aanvaard</v>
+        <v>aanvraag opschorting heffing aanvaard</v>
       </c>
       <c r="G2" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -537,7 +537,7 @@
         <v>aanvraag_opschorting_heffing_niet_aanvaard</v>
       </c>
       <c r="F3" t="str">
-        <v>aanvraag_opschorting_heffing_niet_aanvaard</v>
+        <v>aanvraag opschorting heffing niet aanvaard</v>
       </c>
       <c r="G3" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -596,7 +596,7 @@
         <v>aanvraag_schrapping_aanvaard</v>
       </c>
       <c r="F4" t="str">
-        <v>aanvraag_schrapping_aanvaard</v>
+        <v>aanvraag schrapping aanvaard</v>
       </c>
       <c r="G4" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -655,7 +655,7 @@
         <v>aanvraag_schrapping_niet_aanvaard</v>
       </c>
       <c r="F5" t="str">
-        <v>aanvraag_schrapping_niet_aanvaard</v>
+        <v>aanvraag schrapping niet aanvaard</v>
       </c>
       <c r="G5" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -714,7 +714,7 @@
         <v>beroep_tegen_registratie_ingewilligd</v>
       </c>
       <c r="F6" t="str">
-        <v>beroep_tegen_registratie_ingewilligd</v>
+        <v>beroep tegen registratie ingewilligd</v>
       </c>
       <c r="G6" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -773,7 +773,7 @@
         <v>beroep_tegen_registratie_onontvankelijk_verklaard</v>
       </c>
       <c r="F7" t="str">
-        <v>beroep_tegen_registratie_onontvankelijk_verklaard</v>
+        <v>beroep tegen registratie onontvankelijk verklaard</v>
       </c>
       <c r="G7" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -832,7 +832,7 @@
         <v>beroep_tegen_registratie_verworpen</v>
       </c>
       <c r="F8" t="str">
-        <v>beroep_tegen_registratie_verworpen</v>
+        <v>beroep tegen registratie verworpen</v>
       </c>
       <c r="G8" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -950,7 +950,7 @@
         <v>geschrapt_uit_inventaris</v>
       </c>
       <c r="F10" t="str">
-        <v>geschrapt_uit_inventaris</v>
+        <v>geschrapt uit inventaris</v>
       </c>
       <c r="G10" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1009,7 +1009,7 @@
         <v>heffing_opgeschort</v>
       </c>
       <c r="F11" t="str">
-        <v>heffing_opgeschort</v>
+        <v>heffing opgeschort</v>
       </c>
       <c r="G11" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1127,7 +1127,7 @@
         <v>registratie_ingetrokken</v>
       </c>
       <c r="F13" t="str">
-        <v>registratie_ingetrokken</v>
+        <v>registratie ingetrokken</v>
       </c>
       <c r="G13" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/instumenterend_ambtenaar</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/instrumenterend_ambtenaar</v>
       </c>
       <c r="B20" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2582,7 +2582,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-verwaarlozing</v>
       </c>
       <c r="S37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/curator|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/eigenaar|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/instumenterend_ambtenaar|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/raadsman</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/curator|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/eigenaar|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/instrumenterend_ambtenaar|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/raadsman</v>
       </c>
     </row>
     <row r="38">

</xml_diff>

<commit_message>
LVBR-379 verlenging bij vernieuwing toevoegen aan codelijst
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S44"/>
+  <dimension ref="A1:S45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -699,7 +699,7 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/vernieuwing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/verlenging_bij_vernieuwing</v>
       </c>
       <c r="B6" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -711,10 +711,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/aanvraag_opschorting_heffing_reden</v>
       </c>
       <c r="E6" t="str">
-        <v>vernieuwing</v>
+        <v>verlenging_bij_vernieuwing</v>
       </c>
       <c r="F6" t="str">
-        <v>Vernieuwing, al of niet gekoppeld aan de beëindiging van de leegstand</v>
+        <v>Verlenging bij vernieuwing</v>
       </c>
       <c r="G6" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/aanvraag_opschorting_heffing_reden</v>
@@ -758,7 +758,7 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_aanvaard</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/vernieuwing</v>
       </c>
       <c r="B7" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -767,16 +767,16 @@
         <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_opschorting_heffing</v>
       </c>
       <c r="D7" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/aanvraag_opschorting_heffing_reden</v>
       </c>
       <c r="E7" t="str">
-        <v>aanvraag_opschorting_heffing_aanvaard</v>
+        <v>vernieuwing</v>
       </c>
       <c r="F7" t="str">
-        <v>Aanvraag opschorting heffing aanvaard</v>
+        <v>Vernieuwing, al of niet gekoppeld aan de beëindiging van de leegstand</v>
       </c>
       <c r="G7" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/aanvraag_opschorting_heffing_reden</v>
       </c>
       <c r="H7" t="str">
         <v>null</v>
@@ -817,7 +817,7 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_niet_aanvaard</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_aanvaard</v>
       </c>
       <c r="B8" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -829,10 +829,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E8" t="str">
-        <v>aanvraag_opschorting_heffing_niet_aanvaard</v>
+        <v>aanvraag_opschorting_heffing_aanvaard</v>
       </c>
       <c r="F8" t="str">
-        <v>Aanvraag opschorting heffing niet aanvaard</v>
+        <v>Aanvraag opschorting heffing aanvaard</v>
       </c>
       <c r="G8" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -876,22 +876,22 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_aanvaard</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_niet_aanvaard</v>
       </c>
       <c r="B9" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C9" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_schrapping</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_opschorting_heffing</v>
       </c>
       <c r="D9" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E9" t="str">
-        <v>aanvraag_schrapping_aanvaard</v>
+        <v>aanvraag_opschorting_heffing_niet_aanvaard</v>
       </c>
       <c r="F9" t="str">
-        <v>Aanvraag schrapping aanvaard</v>
+        <v>Aanvraag opschorting heffing niet aanvaard</v>
       </c>
       <c r="G9" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -935,7 +935,7 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_niet_aanvaard</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_aanvaard</v>
       </c>
       <c r="B10" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -947,10 +947,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E10" t="str">
-        <v>aanvraag_schrapping_niet_aanvaard</v>
+        <v>aanvraag_schrapping_aanvaard</v>
       </c>
       <c r="F10" t="str">
-        <v>Aanvraag schrapping niet aanvaard</v>
+        <v>Aanvraag schrapping aanvaard</v>
       </c>
       <c r="G10" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -994,22 +994,22 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_ingewilligd</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_niet_aanvaard</v>
       </c>
       <c r="B11" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C11" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/beroep_tegen_registratie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_schrapping</v>
       </c>
       <c r="D11" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E11" t="str">
-        <v>beroep_tegen_registratie_ingewilligd</v>
+        <v>aanvraag_schrapping_niet_aanvaard</v>
       </c>
       <c r="F11" t="str">
-        <v>Beroep tegen registratie ingewilligd</v>
+        <v>Aanvraag schrapping niet aanvaard</v>
       </c>
       <c r="G11" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_onontvankelijk_verklaard</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_ingewilligd</v>
       </c>
       <c r="B12" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1065,10 +1065,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E12" t="str">
-        <v>beroep_tegen_registratie_onontvankelijk_verklaard</v>
+        <v>beroep_tegen_registratie_ingewilligd</v>
       </c>
       <c r="F12" t="str">
-        <v>Beroep tegen registratie onontvankelijk verklaard</v>
+        <v>Beroep tegen registratie ingewilligd</v>
       </c>
       <c r="G12" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_verworpen</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_onontvankelijk_verklaard</v>
       </c>
       <c r="B13" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1124,10 +1124,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E13" t="str">
-        <v>beroep_tegen_registratie_verworpen</v>
+        <v>beroep_tegen_registratie_onontvankelijk_verklaard</v>
       </c>
       <c r="F13" t="str">
-        <v>Beroep tegen registratie verworpen</v>
+        <v>Beroep tegen registratie onontvankelijk verklaard</v>
       </c>
       <c r="G13" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1171,22 +1171,22 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geregistreerd_in_inventaris</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_verworpen</v>
       </c>
       <c r="B14" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C14" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/registreren</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/beroep_tegen_registratie</v>
       </c>
       <c r="D14" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E14" t="str">
-        <v>geregistreerd_in_inventaris</v>
+        <v>beroep_tegen_registratie_verworpen</v>
       </c>
       <c r="F14" t="str">
-        <v>Geregistreerd in inventaris</v>
+        <v>Beroep tegen registratie verworpen</v>
       </c>
       <c r="G14" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1230,22 +1230,22 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geschrapt_uit_inventaris</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geregistreerd_in_inventaris</v>
       </c>
       <c r="B15" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C15" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/registreren</v>
       </c>
       <c r="D15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E15" t="str">
-        <v>Geschrapt_uit_inventaris</v>
+        <v>geregistreerd_in_inventaris</v>
       </c>
       <c r="F15" t="str">
-        <v>Geschrapt uit inventaris</v>
+        <v>Geregistreerd in inventaris</v>
       </c>
       <c r="G15" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1289,7 +1289,7 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/heffing_opgeschort</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geschrapt_uit_inventaris</v>
       </c>
       <c r="B16" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1301,10 +1301,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E16" t="str">
-        <v>heffing_opgeschort</v>
+        <v>Geschrapt_uit_inventaris</v>
       </c>
       <c r="F16" t="str">
-        <v>Heffing opgeschort</v>
+        <v>Geschrapt uit inventaris</v>
       </c>
       <c r="G16" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1348,22 +1348,22 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/niet_geregistreerd_in_inventaris</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/heffing_opgeschort</v>
       </c>
       <c r="B17" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C17" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/registreren</v>
+        <v>null</v>
       </c>
       <c r="D17" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E17" t="str">
-        <v>niet_geregistreerd_in_inventaris</v>
+        <v>heffing_opgeschort</v>
       </c>
       <c r="F17" t="str">
-        <v>Niet geregistreerd in inventaris</v>
+        <v>Heffing opgeschort</v>
       </c>
       <c r="G17" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1407,22 +1407,22 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/registratie_ingetrokken</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/niet_geregistreerd_in_inventaris</v>
       </c>
       <c r="B18" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C18" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/registreren</v>
       </c>
       <c r="D18" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E18" t="str">
-        <v>registratie_ingetrokken</v>
+        <v>niet_geregistreerd_in_inventaris</v>
       </c>
       <c r="F18" t="str">
-        <v>Registratie ingetrokken</v>
+        <v>Niet geregistreerd in inventaris</v>
       </c>
       <c r="G18" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
@@ -1466,25 +1466,25 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_opschorting_heffing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/registratie_ingetrokken</v>
       </c>
       <c r="B19" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_niet_aanvaard</v>
+        <v>null</v>
       </c>
       <c r="D19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="E19" t="str">
-        <v>null</v>
+        <v>registratie_ingetrokken</v>
       </c>
       <c r="F19" t="str">
-        <v>Aanvraag opschorting heffing</v>
+        <v>Registratie ingetrokken</v>
       </c>
       <c r="G19" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="H19" t="str">
         <v>null</v>
@@ -1525,13 +1525,13 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_schrapping</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_opschorting_heffing</v>
       </c>
       <c r="B20" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C20" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_niet_aanvaard</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_niet_aanvaard</v>
       </c>
       <c r="D20" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
@@ -1540,7 +1540,7 @@
         <v>null</v>
       </c>
       <c r="F20" t="str">
-        <v>Aanvraag schrapping</v>
+        <v>Aanvraag opschorting heffing</v>
       </c>
       <c r="G20" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
@@ -1584,13 +1584,13 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/beroep_tegen_registratie</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_schrapping</v>
       </c>
       <c r="B21" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C21" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_verworpen</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_niet_aanvaard</v>
       </c>
       <c r="D21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
@@ -1599,7 +1599,7 @@
         <v>null</v>
       </c>
       <c r="F21" t="str">
-        <v>Beroep tegen registratie</v>
+        <v>Aanvraag schrapping</v>
       </c>
       <c r="G21" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
@@ -1643,13 +1643,13 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/registreren</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/beroep_tegen_registratie</v>
       </c>
       <c r="B22" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C22" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geregistreerd_in_inventaris|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/niet_geregistreerd_in_inventaris</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_verworpen</v>
       </c>
       <c r="D22" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
@@ -1658,7 +1658,7 @@
         <v>null</v>
       </c>
       <c r="F22" t="str">
-        <v>Registreren</v>
+        <v>Beroep tegen registratie</v>
       </c>
       <c r="G22" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
@@ -1702,25 +1702,25 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/curator</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/registreren</v>
       </c>
       <c r="B23" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C23" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geregistreerd_in_inventaris|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/niet_geregistreerd_in_inventaris</v>
       </c>
       <c r="D23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
       </c>
       <c r="E23" t="str">
         <v>null</v>
       </c>
       <c r="F23" t="str">
-        <v>Curator</v>
+        <v>Registreren</v>
       </c>
       <c r="G23" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
       </c>
       <c r="H23" t="str">
         <v>null</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/eigenaar</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/curator</v>
       </c>
       <c r="B24" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1776,16 +1776,16 @@
         <v>null</v>
       </c>
       <c r="F24" t="str">
-        <v>Eigenaar</v>
+        <v>Curator</v>
       </c>
       <c r="G24" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
       </c>
       <c r="H24" t="str">
-        <v>De houder van een van de volgende zakelijke rechten met betrekking tot een bedrijfsgebouw: de volle eigendom, het recht van opstal of van erfpacht, het vruchtgebruik</v>
+        <v>null</v>
       </c>
       <c r="I24" t="str">
-        <v>De houder van een van de volgende zakelijke rechten met betrekking tot een bedrijfsgebouw: de volle eigendom, het recht van opstal of van erfpacht, het vruchtgebruik</v>
+        <v>null</v>
       </c>
       <c r="J24" t="str">
         <v>null</v>
@@ -1820,7 +1820,7 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/instrumenterend_ambtenaar</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/eigenaar</v>
       </c>
       <c r="B25" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1835,16 +1835,16 @@
         <v>null</v>
       </c>
       <c r="F25" t="str">
-        <v>Instrumenterend ambtenaar</v>
+        <v>Eigenaar</v>
       </c>
       <c r="G25" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
       </c>
       <c r="H25" t="str">
-        <v>Iedere persoon of instelling die ertoe gemachtigd is aktes van eigendomsoverdracht te verlijden</v>
+        <v>De houder van een van de volgende zakelijke rechten met betrekking tot een bedrijfsgebouw: de volle eigendom, het recht van opstal of van erfpacht, het vruchtgebruik</v>
       </c>
       <c r="I25" t="str">
-        <v>Iedere persoon of instelling die ertoe gemachtigd is aktes van eigendomsoverdracht te verlijden</v>
+        <v>De houder van een van de volgende zakelijke rechten met betrekking tot een bedrijfsgebouw: de volle eigendom, het recht van opstal of van erfpacht, het vruchtgebruik</v>
       </c>
       <c r="J25" t="str">
         <v>null</v>
@@ -1879,7 +1879,7 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/raadsman</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/instrumenterend_ambtenaar</v>
       </c>
       <c r="B26" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1894,16 +1894,16 @@
         <v>null</v>
       </c>
       <c r="F26" t="str">
-        <v>Raadsman</v>
+        <v>Instrumenterend ambtenaar</v>
       </c>
       <c r="G26" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
       </c>
       <c r="H26" t="str">
-        <v>null</v>
+        <v>Iedere persoon of instelling die ertoe gemachtigd is aktes van eigendomsoverdracht te verlijden</v>
       </c>
       <c r="I26" t="str">
-        <v>null</v>
+        <v>Iedere persoon of instelling die ertoe gemachtigd is aktes van eigendomsoverdracht te verlijden</v>
       </c>
       <c r="J26" t="str">
         <v>null</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitenmuren</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/raadsman</v>
       </c>
       <c r="B27" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -1947,16 +1947,16 @@
         <v>null</v>
       </c>
       <c r="D27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
       </c>
       <c r="E27" t="str">
-        <v>buitenmuren</v>
+        <v>null</v>
       </c>
       <c r="F27" t="str">
-        <v>Gebrek aan de toestand van buitenmuren</v>
+        <v>Raadsman</v>
       </c>
       <c r="G27" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
       </c>
       <c r="H27" t="str">
         <v>null</v>
@@ -1965,22 +1965,22 @@
         <v>null</v>
       </c>
       <c r="J27" t="str">
-        <v>Buitenmuren</v>
+        <v>null</v>
       </c>
       <c r="K27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>null</v>
       </c>
       <c r="L27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>null</v>
       </c>
       <c r="M27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>null</v>
       </c>
       <c r="N27" t="str">
-        <v>http://www.eionet.europa.eu/gemet/theme/5</v>
+        <v>null</v>
       </c>
       <c r="O27" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_buitenmuren</v>
+        <v>null</v>
       </c>
       <c r="P27" t="str">
         <v>null</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitentimmerwerk</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitenmuren</v>
       </c>
       <c r="B28" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2009,10 +2009,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E28" t="str">
-        <v>buitentimmerwerk</v>
+        <v>buitenmuren</v>
       </c>
       <c r="F28" t="str">
-        <v>Gebrek aan de toestand van het buitentimmerwerk</v>
+        <v>Gebrek aan de toestand van buitenmuren</v>
       </c>
       <c r="G28" t="str">
         <v>null</v>
@@ -2024,7 +2024,7 @@
         <v>null</v>
       </c>
       <c r="J28" t="str">
-        <v>Buitentimmerwerk</v>
+        <v>Buitenmuren</v>
       </c>
       <c r="K28" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
@@ -2039,7 +2039,7 @@
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O28" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_buitentimmerwerk</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_buitenmuren</v>
       </c>
       <c r="P28" t="str">
         <v>null</v>
@@ -2056,7 +2056,7 @@
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakbedekking</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitentimmerwerk</v>
       </c>
       <c r="B29" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2068,10 +2068,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E29" t="str">
-        <v>dakbedekking</v>
+        <v>buitentimmerwerk</v>
       </c>
       <c r="F29" t="str">
-        <v>Gebrek aan de toestand van de dakbedekking</v>
+        <v>Gebrek aan de toestand van het buitentimmerwerk</v>
       </c>
       <c r="G29" t="str">
         <v>null</v>
@@ -2083,7 +2083,7 @@
         <v>null</v>
       </c>
       <c r="J29" t="str">
-        <v>Dakbedekking</v>
+        <v>Buitentimmerwerk</v>
       </c>
       <c r="K29" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
@@ -2098,7 +2098,7 @@
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O29" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakbedekking</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_buitentimmerwerk</v>
       </c>
       <c r="P29" t="str">
         <v>null</v>
@@ -2115,7 +2115,7 @@
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgebinte</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakbedekking</v>
       </c>
       <c r="B30" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2127,10 +2127,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E30" t="str">
-        <v>dakgebinte</v>
+        <v>dakbedekking</v>
       </c>
       <c r="F30" t="str">
-        <v>Gebrek aan de toestand van het dakgebinte</v>
+        <v>Gebrek aan de toestand van de dakbedekking</v>
       </c>
       <c r="G30" t="str">
         <v>null</v>
@@ -2142,7 +2142,7 @@
         <v>null</v>
       </c>
       <c r="J30" t="str">
-        <v>Dakgebinte</v>
+        <v>Dakbedekking</v>
       </c>
       <c r="K30" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
@@ -2157,7 +2157,7 @@
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O30" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakgebinte</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakbedekking</v>
       </c>
       <c r="P30" t="str">
         <v>null</v>
@@ -2174,7 +2174,7 @@
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgoten</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgebinte</v>
       </c>
       <c r="B31" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2186,10 +2186,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E31" t="str">
-        <v>dakgoten</v>
+        <v>dakgebinte</v>
       </c>
       <c r="F31" t="str">
-        <v>Gebrek aan de toestand van de dakgoten</v>
+        <v>Gebrek aan de toestand van het dakgebinte</v>
       </c>
       <c r="G31" t="str">
         <v>null</v>
@@ -2201,7 +2201,7 @@
         <v>null</v>
       </c>
       <c r="J31" t="str">
-        <v>Dakgoten</v>
+        <v>Dakgebinte</v>
       </c>
       <c r="K31" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
@@ -2216,7 +2216,7 @@
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O31" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakgoten</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakgebinte</v>
       </c>
       <c r="P31" t="str">
         <v>null</v>
@@ -2233,7 +2233,7 @@
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgoten</v>
       </c>
       <c r="B32" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2245,13 +2245,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E32" t="str">
-        <v>gebouwonderdeel</v>
+        <v>dakgoten</v>
       </c>
       <c r="F32" t="str">
-        <v>Gebrek aan de toestand van een gebouwonderdeel</v>
+        <v>Gebrek aan de toestand van de dakgoten</v>
       </c>
       <c r="G32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
+        <v>null</v>
       </c>
       <c r="H32" t="str">
         <v>null</v>
@@ -2260,28 +2260,28 @@
         <v>null</v>
       </c>
       <c r="J32" t="str">
-        <v>Gebrek aan de toestand van een gebouwonderdeel</v>
+        <v>Dakgoten</v>
       </c>
       <c r="K32" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="L32" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="M32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/liften|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/trappen</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="N32" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_gebouwonderdeel</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_dakgoten</v>
       </c>
       <c r="P32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/liften|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/trappen</v>
+        <v>null</v>
       </c>
       <c r="Q32" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/liften|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/trappen</v>
+        <v>null</v>
       </c>
       <c r="R32" t="str">
         <v>null</v>
@@ -2292,7 +2292,7 @@
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/kroonlijst</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="B33" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2304,13 +2304,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E33" t="str">
-        <v>kroonlijst</v>
+        <v>gebouwonderdeel</v>
       </c>
       <c r="F33" t="str">
-        <v>Gebrek aan de toestand van de kroonlijst</v>
+        <v>Gebrek aan de toestand van een gebouwonderdeel</v>
       </c>
       <c r="G33" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="H33" t="str">
         <v>null</v>
@@ -2319,28 +2319,28 @@
         <v>null</v>
       </c>
       <c r="J33" t="str">
-        <v>Kroonlijst</v>
+        <v>Gebrek aan de toestand van een gebouwonderdeel</v>
       </c>
       <c r="K33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>null</v>
       </c>
       <c r="L33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>null</v>
       </c>
       <c r="M33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/liften|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/trappen</v>
       </c>
       <c r="N33" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O33" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_kroonlijst</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_gebouwonderdeel</v>
       </c>
       <c r="P33" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/liften|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/trappen</v>
       </c>
       <c r="Q33" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitenmuren|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/buitentimmerwerk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakbedekking|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgebinte|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/dakgoten|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/kroonlijst|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/liften|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/schoorstenen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/trappen</v>
       </c>
       <c r="R33" t="str">
         <v>null</v>
@@ -2351,7 +2351,7 @@
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/liften</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/kroonlijst</v>
       </c>
       <c r="B34" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2363,10 +2363,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E34" t="str">
-        <v>liften</v>
+        <v>kroonlijst</v>
       </c>
       <c r="F34" t="str">
-        <v>Gebrek aan de toestand van de liften</v>
+        <v>Gebrek aan de toestand van de kroonlijst</v>
       </c>
       <c r="G34" t="str">
         <v>null</v>
@@ -2378,7 +2378,7 @@
         <v>null</v>
       </c>
       <c r="J34" t="str">
-        <v>Liften</v>
+        <v>Kroonlijst</v>
       </c>
       <c r="K34" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
@@ -2393,7 +2393,7 @@
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O34" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_liften</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_kroonlijst</v>
       </c>
       <c r="P34" t="str">
         <v>null</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/schoorstenen</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/liften</v>
       </c>
       <c r="B35" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2422,10 +2422,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E35" t="str">
-        <v>schoorstenen</v>
+        <v>liften</v>
       </c>
       <c r="F35" t="str">
-        <v>Gebrek aan de toestand van schoorstenen</v>
+        <v>Gebrek aan de toestand van de liften</v>
       </c>
       <c r="G35" t="str">
         <v>null</v>
@@ -2437,7 +2437,7 @@
         <v>null</v>
       </c>
       <c r="J35" t="str">
-        <v>Schoorstenen</v>
+        <v>Liften</v>
       </c>
       <c r="K35" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
@@ -2452,7 +2452,7 @@
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O35" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_schoorstenen</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_liften</v>
       </c>
       <c r="P35" t="str">
         <v>null</v>
@@ -2469,7 +2469,7 @@
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/stabiliteit</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/schoorstenen</v>
       </c>
       <c r="B36" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2481,13 +2481,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E36" t="str">
-        <v>stabiliteit</v>
+        <v>schoorstenen</v>
       </c>
       <c r="F36" t="str">
-        <v>Gebrek dat stabiliteit in het gedrang brengt</v>
+        <v>Gebrek aan de toestand van schoorstenen</v>
       </c>
       <c r="G36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
+        <v>null</v>
       </c>
       <c r="H36" t="str">
         <v>null</v>
@@ -2496,22 +2496,22 @@
         <v>null</v>
       </c>
       <c r="J36" t="str">
-        <v>Gebrek dat stabiliteit in het gedrang brengt</v>
+        <v>Schoorstenen</v>
       </c>
       <c r="K36" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="L36" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="M36" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="N36" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O36" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_stabiliteit</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_schoorstenen</v>
       </c>
       <c r="P36" t="str">
         <v>null</v>
@@ -2528,7 +2528,7 @@
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/trappen</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/stabiliteit</v>
       </c>
       <c r="B37" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2540,13 +2540,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E37" t="str">
-        <v>trappen</v>
+        <v>stabiliteit</v>
       </c>
       <c r="F37" t="str">
-        <v>Gebrek aan de toestand van de trappen</v>
+        <v>Gebrek dat stabiliteit in het gedrang brengt</v>
       </c>
       <c r="G37" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="H37" t="str">
         <v>null</v>
@@ -2555,22 +2555,22 @@
         <v>null</v>
       </c>
       <c r="J37" t="str">
-        <v>Trappen</v>
+        <v>Gebrek dat stabiliteit in het gedrang brengt</v>
       </c>
       <c r="K37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>null</v>
       </c>
       <c r="L37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>null</v>
       </c>
       <c r="M37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
+        <v>null</v>
       </c>
       <c r="N37" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O37" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_trappen</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_stabiliteit</v>
       </c>
       <c r="P37" t="str">
         <v>null</v>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="38">
       <c r="A38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/veiligheid</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/trappen</v>
       </c>
       <c r="B38" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2599,13 +2599,13 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E38" t="str">
-        <v>veiligheid</v>
+        <v>trappen</v>
       </c>
       <c r="F38" t="str">
-        <v>Gebrek dat veiligheid in het gedrang brengt</v>
+        <v>Gebrek aan de toestand van de trappen</v>
       </c>
       <c r="G38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
+        <v>null</v>
       </c>
       <c r="H38" t="str">
         <v>null</v>
@@ -2614,22 +2614,22 @@
         <v>null</v>
       </c>
       <c r="J38" t="str">
-        <v>Gebrek dat veiligheid in het gedrang brengt</v>
+        <v>Trappen</v>
       </c>
       <c r="K38" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="L38" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="M38" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel</v>
       </c>
       <c r="N38" t="str">
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O38" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_veiligheid</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_trappen</v>
       </c>
       <c r="P38" t="str">
         <v>null</v>
@@ -2646,7 +2646,7 @@
     </row>
     <row r="39">
       <c r="A39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/vochtindringing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/veiligheid</v>
       </c>
       <c r="B39" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2658,10 +2658,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E39" t="str">
-        <v>vochtindringing</v>
+        <v>veiligheid</v>
       </c>
       <c r="F39" t="str">
-        <v>Gebrek dat leidt tot vochtindringing</v>
+        <v>Gebrek dat veiligheid in het gedrang brengt</v>
       </c>
       <c r="G39" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
@@ -2673,7 +2673,7 @@
         <v>null</v>
       </c>
       <c r="J39" t="str">
-        <v>Gebrek dat leidt tot vochtindringing</v>
+        <v>Gebrek dat veiligheid in het gedrang brengt</v>
       </c>
       <c r="K39" t="str">
         <v>null</v>
@@ -2688,7 +2688,7 @@
         <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O39" t="str">
-        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_vochtindringing</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_veiligheid</v>
       </c>
       <c r="P39" t="str">
         <v>null</v>
@@ -2705,34 +2705,34 @@
     </row>
     <row r="40">
       <c r="A40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/aanvraag_opschorting_heffing_reden</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/vochtindringing</v>
       </c>
       <c r="B40" t="str">
-        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+        <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C40" t="str">
         <v>null</v>
       </c>
       <c r="D40" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="E40" t="str">
-        <v>cs_aanvraag_opschorting_heffing_reden</v>
+        <v>vochtindringing</v>
       </c>
       <c r="F40" t="str">
-        <v>Conceptschema over reden voor een procedure aanvraag opschorting heffing</v>
+        <v>Gebrek dat leidt tot vochtindringing</v>
       </c>
       <c r="G40" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
       </c>
       <c r="H40" t="str">
-        <v>Conceptschema over reden voor een procedure aanvraag opschorting heffing</v>
+        <v>null</v>
       </c>
       <c r="I40" t="str">
-        <v>Conceptschema over reden voor een procedure aanvraag opschorting heffing</v>
+        <v>null</v>
       </c>
       <c r="J40" t="str">
-        <v>null</v>
+        <v>Gebrek dat leidt tot vochtindringing</v>
       </c>
       <c r="K40" t="str">
         <v>null</v>
@@ -2744,10 +2744,10 @@
         <v>null</v>
       </c>
       <c r="N40" t="str">
-        <v>null</v>
+        <v>http://www.eionet.europa.eu/gemet/theme/5</v>
       </c>
       <c r="O40" t="str">
-        <v>null</v>
+        <v>https://data.omgeving.vlaanderen.be/ns/verwaarlozing#vertoont_gebrek_ivm_vochtindringing</v>
       </c>
       <c r="P40" t="str">
         <v>null</v>
@@ -2756,15 +2756,15 @@
         <v>null</v>
       </c>
       <c r="R40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-verwaarlozing</v>
+        <v>null</v>
       </c>
       <c r="S40" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/bodemsaneringsproject|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/brownfieldconvenant|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/leegstaand_niet_verwaarloosd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/nieuwe_eigenaars|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/vernieuwing</v>
+        <v>null</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/aanvraag_opschorting_heffing_reden</v>
       </c>
       <c r="B41" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -2776,19 +2776,19 @@
         <v>null</v>
       </c>
       <c r="E41" t="str">
-        <v>cs_beslissing</v>
+        <v>cs_aanvraag_opschorting_heffing_reden</v>
       </c>
       <c r="F41" t="str">
-        <v>Conceptschema over beslissingen die genomen kunnen worden binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over reden voor een procedure aanvraag opschorting heffing</v>
       </c>
       <c r="G41" t="str">
         <v>null</v>
       </c>
       <c r="H41" t="str">
-        <v>Conceptschema over beslissingen die genomen kunnen worden binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over reden voor een procedure aanvraag opschorting heffing</v>
       </c>
       <c r="I41" t="str">
-        <v>Conceptschema over beslissingen die genomen kunnen worden binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over reden voor een procedure aanvraag opschorting heffing</v>
       </c>
       <c r="J41" t="str">
         <v>null</v>
@@ -2803,7 +2803,7 @@
         <v>null</v>
       </c>
       <c r="N41" t="str">
-        <v>http://www.eionet.europa.eu/gemet/theme/5</v>
+        <v>null</v>
       </c>
       <c r="O41" t="str">
         <v>null</v>
@@ -2818,12 +2818,12 @@
         <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-verwaarlozing</v>
       </c>
       <c r="S41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_verworpen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geregistreerd_in_inventaris|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geschrapt_uit_inventaris|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/heffing_opgeschort|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/niet_geregistreerd_in_inventaris|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/registratie_ingetrokken</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/bodemsaneringsproject|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/brownfieldconvenant|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/leegstaand_niet_verwaarloosd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/nieuwe_eigenaars|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/verlenging_bij_vernieuwing|https://data.omgeving.vlaanderen.be/id/concept/leegstand/aanvraag_opschorting_heffing_reden/vernieuwing</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/beslissing</v>
       </c>
       <c r="B42" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -2835,19 +2835,19 @@
         <v>null</v>
       </c>
       <c r="E42" t="str">
-        <v>cs_procedure</v>
+        <v>cs_beslissing</v>
       </c>
       <c r="F42" t="str">
-        <v>Conceptschema over procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over beslissingen die genomen kunnen worden binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="G42" t="str">
         <v>null</v>
       </c>
       <c r="H42" t="str">
-        <v>Conceptschema over procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over beslissingen die genomen kunnen worden binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="I42" t="str">
-        <v>Conceptschema over procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over beslissingen die genomen kunnen worden binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="J42" t="str">
         <v>null</v>
@@ -2877,12 +2877,12 @@
         <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-verwaarlozing</v>
       </c>
       <c r="S42" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_opschorting_heffing|https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_schrapping|https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/beroep_tegen_registratie|https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/registreren</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_opschorting_heffing_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/aanvraag_schrapping_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/beroep_tegen_registratie_verworpen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geregistreerd_in_inventaris|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/geschrapt_uit_inventaris|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/heffing_opgeschort|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/niet_geregistreerd_in_inventaris|https://data.omgeving.vlaanderen.be/id/concept/leegstand/beslissing/registratie_ingetrokken</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/procedure</v>
       </c>
       <c r="B43" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -2894,19 +2894,19 @@
         <v>null</v>
       </c>
       <c r="E43" t="str">
-        <v>cs_rol</v>
+        <v>cs_procedure</v>
       </c>
       <c r="F43" t="str">
-        <v>Conceptschema over rollen van agenten binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="G43" t="str">
         <v>null</v>
       </c>
       <c r="H43" t="str">
-        <v>Conceptschema over rollen van agenten binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="I43" t="str">
-        <v>Conceptschema over rollen van agenten binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
+        <v>Conceptschema over procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="J43" t="str">
         <v>null</v>
@@ -2936,12 +2936,12 @@
         <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-verwaarlozing</v>
       </c>
       <c r="S43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/curator|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/eigenaar|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/instrumenterend_ambtenaar|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/raadsman</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_opschorting_heffing|https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/aanvraag_schrapping|https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/beroep_tegen_registratie|https://data.omgeving.vlaanderen.be/id/concept/leegstand/procedure/registreren</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/rol</v>
       </c>
       <c r="B44" t="str">
         <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
@@ -2953,19 +2953,19 @@
         <v>null</v>
       </c>
       <c r="E44" t="str">
-        <v>cs_uitgesproken_gebrek</v>
+        <v>cs_rol</v>
       </c>
       <c r="F44" t="str">
-        <v>Conceptschema over kenmerken van verwaarlozing aan gebouwen.</v>
+        <v>Conceptschema over rollen van agenten binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="G44" t="str">
         <v>null</v>
       </c>
       <c r="H44" t="str">
-        <v>Het vertonen van uitgesproken gebreken van algemene of beperkte omvang van bedrijfsverwaarlozing. De Vlaamse regering bepaalt de gebreken van algemene en beperkte omvang, alsook de criteria voor de beoordeling van de gebreken en de minimumnorm van de te vertonen gebreken om een bedrijfsruimte al dan niet als geheel of gedeeltelijk verwaarloosd te beschouwen;</v>
+        <v>Conceptschema over rollen van agenten binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="I44" t="str">
-        <v>Het vertonen van uitgesproken gebreken van algemene of beperkte omvang van bedrijfsverwaarlozing. De Vlaamse regering bepaalt de gebreken van algemene en beperkte omvang, alsook de criteria voor de beoordeling van de gebreken en de minimumnorm van de te vertonen gebreken om een bedrijfsruimte al dan niet als geheel of gedeeltelijk verwaarloosd te beschouwen;</v>
+        <v>Conceptschema over rollen van agenten binnen procedures in het kader van leegstaande en verwaarloosde bedrijfsruimten.</v>
       </c>
       <c r="J44" t="str">
         <v>null</v>
@@ -2995,12 +2995,71 @@
         <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-verwaarlozing</v>
       </c>
       <c r="S44" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/curator|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/eigenaar|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/instrumenterend_ambtenaar|https://data.omgeving.vlaanderen.be/id/concept/leegstand/rol/raadsman</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/uitgesproken_gebrek</v>
+      </c>
+      <c r="B45" t="str">
+        <v>http://www.w3.org/2004/02/skos/core#ConceptScheme</v>
+      </c>
+      <c r="C45" t="str">
+        <v>null</v>
+      </c>
+      <c r="D45" t="str">
+        <v>null</v>
+      </c>
+      <c r="E45" t="str">
+        <v>cs_uitgesproken_gebrek</v>
+      </c>
+      <c r="F45" t="str">
+        <v>Conceptschema over kenmerken van verwaarlozing aan gebouwen.</v>
+      </c>
+      <c r="G45" t="str">
+        <v>null</v>
+      </c>
+      <c r="H45" t="str">
+        <v>Het vertonen van uitgesproken gebreken van algemene of beperkte omvang van bedrijfsverwaarlozing. De Vlaamse regering bepaalt de gebreken van algemene en beperkte omvang, alsook de criteria voor de beoordeling van de gebreken en de minimumnorm van de te vertonen gebreken om een bedrijfsruimte al dan niet als geheel of gedeeltelijk verwaarloosd te beschouwen;</v>
+      </c>
+      <c r="I45" t="str">
+        <v>Het vertonen van uitgesproken gebreken van algemene of beperkte omvang van bedrijfsverwaarlozing. De Vlaamse regering bepaalt de gebreken van algemene en beperkte omvang, alsook de criteria voor de beoordeling van de gebreken en de minimumnorm van de te vertonen gebreken om een bedrijfsruimte al dan niet als geheel of gedeeltelijk verwaarloosd te beschouwen;</v>
+      </c>
+      <c r="J45" t="str">
+        <v>null</v>
+      </c>
+      <c r="K45" t="str">
+        <v>null</v>
+      </c>
+      <c r="L45" t="str">
+        <v>null</v>
+      </c>
+      <c r="M45" t="str">
+        <v>null</v>
+      </c>
+      <c r="N45" t="str">
+        <v>http://www.eionet.europa.eu/gemet/theme/5</v>
+      </c>
+      <c r="O45" t="str">
+        <v>null</v>
+      </c>
+      <c r="P45" t="str">
+        <v>null</v>
+      </c>
+      <c r="Q45" t="str">
+        <v>null</v>
+      </c>
+      <c r="R45" t="str">
+        <v>https://data.omgeving.vlaanderen.be/id/dataset/codelijst-verwaarlozing</v>
+      </c>
+      <c r="S45" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/gebouwonderdeel|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/stabiliteit|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/veiligheid|https://data.omgeving.vlaanderen.be/id/concept/leegstand/uitgesproken_gebrek/vochtindringing</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:S44"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:S45"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LVBR-297 lijst aanpassingen ten gevolge van aligneren met lvbr
</commit_message>
<xml_diff>
--- a/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
+++ b/src/main/resources/be/vlaanderen/omgeving/data/id/conceptscheme/verwaarlozing/verwaarlozing.xlsx
@@ -2012,7 +2012,7 @@
         <v>OPSCH_ANVRD</v>
       </c>
       <c r="F28" t="str">
-        <v>Opschorting aanvaard beslissingsstuk</v>
+        <v>Opschorting aanvaard</v>
       </c>
       <c r="G28" t="str">
         <v>null</v>
@@ -2071,7 +2071,7 @@
         <v>OPSCH_ANVRD_BEG_BRIEF</v>
       </c>
       <c r="F29" t="str">
-        <v>Begeleidende brief bij opschorting aanvaard beslissingsstuk</v>
+        <v>Begeleidende brief bij opschorting aanvaard</v>
       </c>
       <c r="G29" t="str">
         <v>null</v>
@@ -2130,7 +2130,7 @@
         <v>OPSCH_NANVRD</v>
       </c>
       <c r="F30" t="str">
-        <v>Opschorting niet aanvaard beslissingsstuk</v>
+        <v>Opschorting niet aanvaard</v>
       </c>
       <c r="G30" t="str">
         <v>null</v>
@@ -2189,7 +2189,7 @@
         <v>OPSCH_NANVRD_BEG_BRIEF</v>
       </c>
       <c r="F31" t="str">
-        <v>Begeleidende brief bij opschorting niet aanvaard beslissingsstuk</v>
+        <v>Begeleidende brief bij opschorting niet aanvaard</v>
       </c>
       <c r="G31" t="str">
         <v>null</v>
@@ -2248,7 +2248,7 @@
         <v>SCHR_ANVRD</v>
       </c>
       <c r="F32" t="str">
-        <v>Schrapping aanvaard beslissingsstuk</v>
+        <v>Schrapping aanvaard</v>
       </c>
       <c r="G32" t="str">
         <v>null</v>
@@ -2307,7 +2307,7 @@
         <v>SCHR_NANVRD</v>
       </c>
       <c r="F33" t="str">
-        <v>Schrapping niet aanvaard beslissingsstuk</v>
+        <v>Schrapping niet aanvaard</v>
       </c>
       <c r="G33" t="str">
         <v>null</v>
@@ -2366,7 +2366,7 @@
         <v>SCHR_NANVRD_BEG_BRIEF</v>
       </c>
       <c r="F34" t="str">
-        <v>Begeleidende brief bij schrapping niet aanvaard beslissingsstuk</v>
+        <v>Begeleidende brief bij schrapping niet aanvaard</v>
       </c>
       <c r="G34" t="str">
         <v>null</v>
@@ -2425,7 +2425,7 @@
         <v>BER_INGWD</v>
       </c>
       <c r="F35" t="str">
-        <v>Beroep ingewilligd beslissingsstuk</v>
+        <v>Beroep ingewilligd</v>
       </c>
       <c r="G35" t="str">
         <v>null</v>
@@ -2484,7 +2484,7 @@
         <v>BER_INGWD_BEG_BRIEF</v>
       </c>
       <c r="F36" t="str">
-        <v>Begeleidende brief bij beroep ingewilligd beslissingsstuk</v>
+        <v>Begeleidende brief bij beroep ingewilligd</v>
       </c>
       <c r="G36" t="str">
         <v>null</v>
@@ -2543,7 +2543,7 @@
         <v>BER_ON</v>
       </c>
       <c r="F37" t="str">
-        <v>Beroep onontvankelijk beslissingsstuk</v>
+        <v>Beroep onontvankelijk verklaard</v>
       </c>
       <c r="G37" t="str">
         <v>null</v>
@@ -2602,7 +2602,7 @@
         <v>BER_ON_BEG_BRIEF</v>
       </c>
       <c r="F38" t="str">
-        <v>Begeleidende brief bij beroep onontvankelijk beslissingsstuk</v>
+        <v>Begeleidende brief bij beroep onontvankelijk verklaard</v>
       </c>
       <c r="G38" t="str">
         <v>null</v>
@@ -2661,7 +2661,7 @@
         <v>BER_VERWN</v>
       </c>
       <c r="F39" t="str">
-        <v>Beroep verworpen beslissingsstuk</v>
+        <v>Beroep verworpen</v>
       </c>
       <c r="G39" t="str">
         <v>null</v>
@@ -2720,7 +2720,7 @@
         <v>BER_VERWN_BEG_BRIEF</v>
       </c>
       <c r="F40" t="str">
-        <v>Begeleidende brief bij beroep verworpen beslissingsstuk</v>
+        <v>Begeleidende brief bij beroep verworpen</v>
       </c>
       <c r="G40" t="str">
         <v>null</v>
@@ -2797,13 +2797,13 @@
         <v>null</v>
       </c>
       <c r="L41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/schrapping_aanvaard_begeleidende_brief</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratieattest|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratieattest_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/schrapping_aanvaard_begeleidende_brief</v>
       </c>
       <c r="M41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/schrapping_aanvaard_begeleidende_brief</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratieattest|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratieattest_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/schrapping_aanvaard_begeleidende_brief</v>
       </c>
       <c r="N41" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/schrapping_aanvaard_begeleidende_brief</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_opschorting_heffing_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/aanvraag_schrapping_niet_aanvaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_ingewilligd_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_onontvankelijk_verklaard_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/beroep_tegen_registratie_verworpen_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratieattest|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratieattest_begeleidende_brief|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/schrapping_aanvaard_begeleidende_brief</v>
       </c>
       <c r="O41" t="str">
         <v>null</v>
@@ -2882,7 +2882,7 @@
     </row>
     <row r="43">
       <c r="A43" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/procedure_inkomend_stuk</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/inkomend_procedurestuk</v>
       </c>
       <c r="B43" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -2894,10 +2894,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/stuk</v>
       </c>
       <c r="E43" t="str">
-        <v>PRO_INKOMEND_STUK</v>
+        <v>INKOMEND_PROCEDURESTUK</v>
       </c>
       <c r="F43" t="str">
-        <v>Inkomend stuk op een procedure</v>
+        <v>Inkomend procedurestuk</v>
       </c>
       <c r="G43" t="str">
         <v>null</v>
@@ -2974,13 +2974,13 @@
         <v>null</v>
       </c>
       <c r="L44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/procedure_inkomend_stuk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/retour_afzender</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/inkomend_procedurestuk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/retour_afzender_procedurestuk</v>
       </c>
       <c r="M44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/procedure_inkomend_stuk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/retour_afzender</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/inkomend_procedurestuk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/retour_afzender_procedurestuk</v>
       </c>
       <c r="N44" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/procedure_inkomend_stuk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/retour_afzender</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/inkomend_procedurestuk|https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/retour_afzender_procedurestuk</v>
       </c>
       <c r="O44" t="str">
         <v>null</v>
@@ -3000,7 +3000,7 @@
     </row>
     <row r="45">
       <c r="A45" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratieattest</v>
       </c>
       <c r="B45" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3012,10 +3012,10 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/stuk</v>
       </c>
       <c r="E45" t="str">
-        <v>REG_ATT</v>
+        <v>REGATT</v>
       </c>
       <c r="F45" t="str">
-        <v>Registratie attest</v>
+        <v>Registratieattest</v>
       </c>
       <c r="G45" t="str">
         <v>null</v>
@@ -3059,22 +3059,22 @@
     </row>
     <row r="46">
       <c r="A46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest_begeleidende_brief</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratieattest_begeleidende_brief</v>
       </c>
       <c r="B46" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
       </c>
       <c r="C46" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/registratie_attest</v>
+        <v>null</v>
       </c>
       <c r="D46" t="str">
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/stuk</v>
       </c>
       <c r="E46" t="str">
-        <v>REG_ATT_BEG_BRIEF</v>
+        <v>REGATT_BEG_BRIEF</v>
       </c>
       <c r="F46" t="str">
-        <v>Begeleidende brief bij een registratie attest</v>
+        <v>Begeleidende brief bij een registratieattest</v>
       </c>
       <c r="G46" t="str">
         <v>null</v>
@@ -3118,7 +3118,7 @@
     </row>
     <row r="47">
       <c r="A47" t="str">
-        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/retour_afzender</v>
+        <v>https://data.omgeving.vlaanderen.be/id/concept/leegstand/stuk/retour_afzender_procedurestuk</v>
       </c>
       <c r="B47" t="str">
         <v>http://www.w3.org/2004/02/skos/core#Concept</v>
@@ -3130,7 +3130,7 @@
         <v>https://data.omgeving.vlaanderen.be/id/conceptscheme/leegstand/stuk</v>
       </c>
       <c r="E47" t="str">
-        <v>RETOUR_AFZENDER</v>
+        <v>RETOUR_AFZENDER_PROCEDURESTUK</v>
       </c>
       <c r="F47" t="str">
         <v>Retour afzender</v>
@@ -3192,7 +3192,7 @@
         <v>SCHR_ANVRD_BEG_BRIEF</v>
       </c>
       <c r="F48" t="str">
-        <v>Begeleidende brief bij schrapping aanvaard beslissingsstuk</v>
+        <v>Begeleidende brief bij schrapping aanvaard</v>
       </c>
       <c r="G48" t="str">
         <v>null</v>

</xml_diff>